<commit_message>
adjusted for flash delivery | new excel format (temp & remaining)
</commit_message>
<xml_diff>
--- a/source-code/python-code/support-files/เช็คยอด-COD.xlsx
+++ b/source-code/python-code/support-files/เช็คยอด-COD.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>วันที่ส่งพัสดุ</t>
   </si>
   <si>
-    <t>เลขที่ AWB</t>
-  </si>
-  <si>
     <t>ผู้รับ</t>
   </si>
   <si>
@@ -29,13 +26,19 @@
   </si>
   <si>
     <t>สถานะ</t>
+  </si>
+  <si>
+    <t>Tracking Number</t>
+  </si>
+  <si>
+    <t>Tel.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,15 +49,23 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="arial"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="arial"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -121,11 +132,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +442,7 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -440,31 +451,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="55.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>